<commit_message>
Added new users in the questionnaires. Doodle updated
</commit_message>
<xml_diff>
--- a/Forms/AfterTest (respostas).xlsx
+++ b/Forms/AfterTest (respostas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="291">
   <si>
     <t>Indicação de data e hora</t>
   </si>
@@ -761,6 +761,129 @@
   </si>
   <si>
     <t>Aline</t>
+  </si>
+  <si>
+    <t>Ação mais fácil</t>
+  </si>
+  <si>
+    <t>Ação super fácil também</t>
+  </si>
+  <si>
+    <t>A falta da perspectiva faz com que necessite rotacionar a camera, o que é muito ruim quando outras ações estão sendo realizadas.</t>
+  </si>
+  <si>
+    <t>Bernardo Henz</t>
+  </si>
+  <si>
+    <t>Vinícius Breda</t>
+  </si>
+  <si>
+    <t>Não houve muita estratégia. O papel de cada player foi bem dinâmico.</t>
+  </si>
+  <si>
+    <t>Em geral, achei bacana. Só acho que, para obter melhor precisão nas tarefas, deveria haver um tipo melhor de feedback, como por exemplo, uma indicação de punição caso o cubo não esteja ocupando bem o volume dos obstáculos.</t>
+  </si>
+  <si>
+    <t>Jonas Deyson</t>
+  </si>
+  <si>
+    <t>O fato de ter de usar as duas mãos torna menos confortável fazer a escala</t>
+  </si>
+  <si>
+    <t>Não houve divisão combinada. Cada um fez o que achava que devesse fazer, e acabou dando certo. Mas alguns acabaram se concentrando em algumas tarefas mais do que outros, como escala, translação e rotação de câmera.</t>
+  </si>
+  <si>
+    <t>A rotação acaba sendo um pouco desconfortável para o pulso, mas nada que prejudique muito.</t>
+  </si>
+  <si>
+    <t>Alex Reimann Cunha Lima</t>
+  </si>
+  <si>
+    <t>Cada um ficou com uma única ação.</t>
+  </si>
+  <si>
+    <t>Gostei muito da experiência.</t>
+  </si>
+  <si>
+    <t>Mariane Giambastiani</t>
+  </si>
+  <si>
+    <t>Na minha opinião a representação do celular atrapalhou a visibilidade do cubo</t>
+  </si>
+  <si>
+    <t>Cada um ficou com uma tarefa diferente</t>
+  </si>
+  <si>
+    <t>A experiência em si foi legal, não exigiu demais, mas também não foi "estúpido", minha única crítica é a representação dos celulares mesmo que às vezes ficavam na frente do cubo.</t>
+  </si>
+  <si>
+    <t>Tatiane Sequerra Stivelman</t>
+  </si>
+  <si>
+    <t>Intuitivo para àqueles que têm noções de 3D, já que é necessário mover o celular para o plano que desejas mover o objeto.</t>
+  </si>
+  <si>
+    <t>O mesmo que da ação de translação.</t>
+  </si>
+  <si>
+    <t>Muito fácil e simples.</t>
+  </si>
+  <si>
+    <t>Uma ação muito útil e de fácil manipulação.</t>
+  </si>
+  <si>
+    <t>Cada um dos jogadores ficou responsável por uma ação e cada um realizava sua respectiva função quando necessária.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achei muito interessante o trabalho, principalmente pela mobilidade que é proporcionada através do uso de smartphones (com compatibilidade de sistema operacional). O jogo, se é assim que posso me referir, é independente à widgets e outras ferramentas fechadas. Os movimentos do celular são muito intuitivos e isso facilita a realização das tarefas, já que grande maioria das pessoas já estão habituadas a tais movimentos. </t>
+  </si>
+  <si>
+    <t>Mathias Fassini Mantelli</t>
+  </si>
+  <si>
+    <t>Em geral sou canhota e isso dificultou o manuseio do celular por ser com a mão direita. Talvez fosse interessante que todos os comandos ficassem na tela como um joystick.</t>
+  </si>
+  <si>
+    <t>Mesma situação da rotação do objeto.</t>
+  </si>
+  <si>
+    <t>Talvez tornar a representação do celular menor para facilitar a visualização do objeto trabalhado.</t>
+  </si>
+  <si>
+    <t>Cada um ficou responsável por uma ação e nos comunicávamos durante o jogo solicitando a ação do colega.</t>
+  </si>
+  <si>
+    <t>Nenhum desconforto.</t>
+  </si>
+  <si>
+    <t>Gostei do jogo!</t>
+  </si>
+  <si>
+    <t>Fernanda Caroline Silveira Rodrigues</t>
+  </si>
+  <si>
+    <t>Transladei duas vezes o objeto sem querer, por tirar um dedo mais rápido que o outro durante o processo de escala</t>
+  </si>
+  <si>
+    <t>Conforme ja comentado acima, por tirar um dedo mais rapido que o outro, por duas vezes transladei o objeto sem a intenção ao finalizar uma escala.</t>
+  </si>
+  <si>
+    <t>Diego Pittol</t>
+  </si>
+  <si>
+    <t>Emanuel Novakoski</t>
+  </si>
+  <si>
+    <t>O uso dos botoes de volume eh desconfortavel</t>
+  </si>
+  <si>
+    <t>Muito interessante</t>
+  </si>
+  <si>
+    <t>Mauricio Barbosa da Rocha</t>
+  </si>
+  <si>
+    <t>Maurício Calegari Xavier</t>
   </si>
 </sst>
 </file>
@@ -7233,6 +7356,1602 @@
         <v>249</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" s="3">
+        <v>42531.586675300925</v>
+      </c>
+      <c r="B47" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="C47" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F47" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="I47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="L47" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="M47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="N47" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="P47" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="R47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="S47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="T47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="V47" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W47" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X47" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Y47" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AA47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AB47" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AD47" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AE47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AG47" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AH47" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AI47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP47" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW47" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AX47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA47" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3">
+        <v>42531.58704938657</v>
+      </c>
+      <c r="B48" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="K48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="M48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="O48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="R48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="S48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="T48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="V48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AB48" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AD48" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AE48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AG48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AH48" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AI48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT48" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY48" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA48" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3">
+        <v>42531.5898059375</v>
+      </c>
+      <c r="B49" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="L49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="M49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="N49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="O49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="P49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="R49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="S49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="T49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="V49" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W49" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X49" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AA49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AB49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AD49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AE49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AG49" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AH49" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AI49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL49" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO49" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP49" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR49" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AS49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW49" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AX49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA49" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3">
+        <v>42531.591108865745</v>
+      </c>
+      <c r="B50" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="C50" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F50" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I50" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="L50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="M50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N50" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="P50" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="R50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="S50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="T50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="V50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="W50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="X50" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="Y50" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="Z50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AB50" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AE50" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AG50" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AH50" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AI50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR50" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="AS50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT50" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW50" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="AX50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY50" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA50" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3">
+        <v>42531.7084683912</v>
+      </c>
+      <c r="B51" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="M51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="R51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="S51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="T51" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="V51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="Z51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AA51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AB51" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AD51" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AE51" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AG51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AH51" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AI51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR51" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AS51" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT51" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU51" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW51" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AX51" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY51" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ51" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA51" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3">
+        <v>42531.7087703588</v>
+      </c>
+      <c r="B52" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C52" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K52" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="M52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="O52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="P52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="R52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="S52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="T52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="V52" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W52" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X52" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AA52" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AB52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AD52" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AE52" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AF52" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AG52" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AH52" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AI52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK52" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL52" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO52" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP52" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR52" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="AS52" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT52" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU52" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW52" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AX52" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY52" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ52" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA52" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3">
+        <v>42531.70931443287</v>
+      </c>
+      <c r="B53" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D53" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G53" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="K53" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="M53" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="N53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="O53" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="P53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="Q53" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="R53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="S53" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="T53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="U53" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="V53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="W53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="X53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="Y53" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AB53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AC53" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AE53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AG53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AH53" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AI53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM53" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO53" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP53" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR53" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="AS53" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU53" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW53" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AX53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ53" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA53" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3">
+        <v>42531.710083240745</v>
+      </c>
+      <c r="B54" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F54" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H54" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="K54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="L54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="M54" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="N54" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="O54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="R54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="S54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="T54" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="U54" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="V54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AB54" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AC54" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="AD54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AE54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AF54" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AG54" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AH54" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AI54" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ54" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK54" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL54" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO54" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP54" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR54" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV54" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="AW54" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="AX54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA54" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3">
+        <v>42531.73696648148</v>
+      </c>
+      <c r="B55" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D55" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E55" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F55" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G55" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H55" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J55" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="L55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="M55" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="N55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="O55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="P55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="Q55" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="R55" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="S55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="T55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="V55" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="X55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="Y55" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AB55" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AD55" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AE55" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="BA55" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3">
+        <v>42531.765510173616</v>
+      </c>
+      <c r="B56" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="K56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="M56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="R56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="S56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="T56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="V56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AA56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AB56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AD56" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AE56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AG56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AH56" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AI56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP56" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS56" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY56" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA56" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3">
+        <v>42531.767150960644</v>
+      </c>
+      <c r="B57" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="K57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="M57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="R57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="S57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="T57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="V57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X57" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AB57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AD57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AE57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AG57" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AH57" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AI57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS57" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV57" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="AW57" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AX57" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA57" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3">
+        <v>42531.7810865625</v>
+      </c>
+      <c r="B58" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H58" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="K58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="M58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="N58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="R58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="S58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="T58" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="V58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="W58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="X58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Z58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AA58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AB58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AD58" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AE58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AG58" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="AH58" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AZ58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA58" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>